<commit_message>
update output metabolights assay
</commit_message>
<xml_diff>
--- a/templates/dataplant/3ASY02_ProteomicsMassSpec.xlsx
+++ b/templates/dataplant/3ASY02_ProteomicsMassSpec.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\SWATE_templates\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\Swate-templates_FORK\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E57339-EEC1-43D8-A917-E1556E0C4EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1884452C-6256-461F-9015-EADE526BA1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="19110" windowHeight="12450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6165" yWindow="2340" windowWidth="22785" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3ASY02_ProteomicsMassSpec" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="161">
   <si>
     <t>Source Name</t>
   </si>
@@ -647,6 +647,9 @@
   <si>
     <t>Authors Role Term Source REF</t>
   </si>
+  <si>
+    <t>Raw Data File</t>
+  </si>
 </sst>
 </file>
 
@@ -657,7 +660,7 @@
     <numFmt numFmtId="165" formatCode="0.00\ &quot;count unit&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00\ &quot;second&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -672,12 +675,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -809,7 +806,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -853,6 +850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -977,7 +975,7 @@
     <tableColumn id="34" xr3:uid="{02FFA839-AB2E-4256-AF70-683903B0E222}" name="Unit (#4)" dataDxfId="3"/>
     <tableColumn id="35" xr3:uid="{1DE3AD7A-94C9-4D6D-A620-068505BBA80F}" name="Term Source REF (PATO:0001309)" dataDxfId="2"/>
     <tableColumn id="36" xr3:uid="{89607A56-7C4A-4A91-9B9D-E822F9611BED}" name="Term Accession Number (PATO:0001309)" dataDxfId="1"/>
-    <tableColumn id="37" xr3:uid="{8EFFFFD9-A831-4B22-BB48-207F2316916A}" name="Data File Name" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{F570B6A4-D399-4AE6-A741-7062E131420B}" name="Raw Data File" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1281,7 +1279,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="632" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="630" row="2">
@@ -1314,46 +1312,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="39" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="26.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.5703125" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="37.5703125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30.5703125" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="37.5703125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="30.5703125" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="37.5703125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.140625" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="30.5703125" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="37.5703125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="21.85546875" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="29" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="21.85546875" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="29" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="31" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="30.5703125" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="37.5703125" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="11" hidden="1" customWidth="1"/>
     <col min="34" max="34" width="21.85546875" hidden="1" customWidth="1"/>
     <col min="35" max="35" width="29" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -1463,7 +1463,7 @@
         <v>137</v>
       </c>
       <c r="AJ1" t="s">
-        <v>31</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1548,7 +1548,7 @@
       <c r="AI2" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="AJ2" s="3"/>
+      <c r="AJ2" s="17"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1632,7 +1632,7 @@
       <c r="AI3" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="AJ3" s="3"/>
+      <c r="AJ3" s="17"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -1716,7 +1716,7 @@
       <c r="AI4" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="AJ4" s="3"/>
+      <c r="AJ4" s="17"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1800,7 +1800,7 @@
       <c r="AI5" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="AJ5" s="3"/>
+      <c r="AJ5" s="17"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -1884,7 +1884,7 @@
       <c r="AI6" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="AJ6" s="3"/>
+      <c r="AJ6" s="17"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -1968,7 +1968,7 @@
       <c r="AI7" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="AJ7" s="3"/>
+      <c r="AJ7" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1982,7 +1982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BCA011F-5496-4EB2-AF3E-FA3119C26B5A}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update output proteomics assay
</commit_message>
<xml_diff>
--- a/templates/dataplant/3ASY02_ProteomicsMassSpec.xlsx
+++ b/templates/dataplant/3ASY02_ProteomicsMassSpec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\Swate-templates_FORK\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1884452C-6256-461F-9015-EADE526BA1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9021DC0-6A89-4127-BDFD-62E31601BBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6165" yWindow="2340" windowWidth="22785" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1313,7 +1313,7 @@
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
+      <selection activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>